<commit_message>
commit on 2 march
</commit_message>
<xml_diff>
--- a/4 курс/Информационный менеджмент/Practice4_OIM_Parakhin_PRI120.xlsx
+++ b/4 курс/Информационный менеджмент/Practice4_OIM_Parakhin_PRI120.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="подсчет количественных рисков" sheetId="1" r:id="rId1"/>
+    <sheet name="отчетности" sheetId="2" r:id="rId1"/>
+    <sheet name="трудовые активности" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,49 +20,157 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Риск</t>
-  </si>
-  <si>
-    <t>Разовый ущерб, руб.</t>
-  </si>
-  <si>
-    <t>Частота возникновения, в год</t>
-  </si>
-  <si>
-    <t>Среднегодовой ущерб</t>
-  </si>
-  <si>
-    <t>сбой аппаратного обеспечения</t>
-  </si>
-  <si>
-    <t>сбой программного обеспечения</t>
-  </si>
-  <si>
-    <t>утечка персональных данных</t>
-  </si>
-  <si>
-    <t>порча хранимых данных</t>
-  </si>
-  <si>
-    <t>100 000,00</t>
-  </si>
-  <si>
-    <t>35 000,00</t>
-  </si>
-  <si>
-    <t>50 000,00</t>
-  </si>
-  <si>
-    <t>150 000,00</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+  <si>
+    <t>№ п/п</t>
+  </si>
+  <si>
+    <t>Показатель</t>
+  </si>
+  <si>
+    <t>Предыдущий год</t>
+  </si>
+  <si>
+    <t>План отчётного года</t>
+  </si>
+  <si>
+    <t>Фактически в отчётном году</t>
+  </si>
+  <si>
+    <t>Изменение в процентах к предыдущему году</t>
+  </si>
+  <si>
+    <t>План (гр.2/гр.1*100)</t>
+  </si>
+  <si>
+    <t>Факт (гр.3/гр.1*100)</t>
+  </si>
+  <si>
+    <t>А</t>
+  </si>
+  <si>
+    <t>Б</t>
+  </si>
+  <si>
+    <t>Среднесписочная численность работающих, чел., в том числе:</t>
+  </si>
+  <si>
+    <t>- мужчин</t>
+  </si>
+  <si>
+    <t>- женщин</t>
+  </si>
+  <si>
+    <t>Квалификационный состав, чел., в том числе:</t>
+  </si>
+  <si>
+    <t>- высшее</t>
+  </si>
+  <si>
+    <t>- среднее специальное</t>
+  </si>
+  <si>
+    <t>- среднее профессиональное</t>
+  </si>
+  <si>
+    <t>Распределение работников по категориям работ, чел., из них:</t>
+  </si>
+  <si>
+    <t>ведущий</t>
+  </si>
+  <si>
+    <t>1-я категория</t>
+  </si>
+  <si>
+    <t>2-я категория</t>
+  </si>
+  <si>
+    <t>без категории и т.д.</t>
+  </si>
+  <si>
+    <t>Распределение работников по профессиям, чел., из них:</t>
+  </si>
+  <si>
+    <t>тестировщики</t>
+  </si>
+  <si>
+    <t>бизнес-аналитики</t>
+  </si>
+  <si>
+    <t>программисты</t>
+  </si>
+  <si>
+    <t>Среднегодовая заработная плата</t>
+  </si>
+  <si>
+    <t>Коэффициент интенсивности работы по приему (Кп)</t>
+  </si>
+  <si>
+    <t>Коэффициент работы по выбытию (Кв)</t>
+  </si>
+  <si>
+    <t>Коэффициент текучести (Кт)</t>
+  </si>
+  <si>
+    <t>Коэффициент замещения (Кз)</t>
+  </si>
+  <si>
+    <t>Коэффициент постоянства кадров</t>
+  </si>
+  <si>
+    <t>Производственно-экономические</t>
+  </si>
+  <si>
+    <t>всего разработчиков</t>
+  </si>
+  <si>
+    <t>Уровень выполнения трудовых норм</t>
+  </si>
+  <si>
+    <t>Трудовая дисциплина</t>
+  </si>
+  <si>
+    <t>Среднее</t>
+  </si>
+  <si>
+    <t>Творческая активность</t>
+  </si>
+  <si>
+    <t>Изобретательство</t>
+  </si>
+  <si>
+    <t>Разработка инноваций</t>
+  </si>
+  <si>
+    <t>Значения</t>
+  </si>
+  <si>
+    <t>Развитие личности</t>
+  </si>
+  <si>
+    <t>Повышение квалификации</t>
+  </si>
+  <si>
+    <t>Расширение профессионального профиля</t>
+  </si>
+  <si>
+    <t>Общественная активность в сфере производства</t>
+  </si>
+  <si>
+    <t>Среднее значение при среднем числе разработчиков (равным 20)</t>
+  </si>
+  <si>
+    <t>Участие в выработке и принятии технологических решений</t>
+  </si>
+  <si>
+    <t>Участие в управлении проектами разработки</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,16 +190,58 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE599"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD1F1DA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDE49B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF34A853"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -150,11 +301,155 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -163,16 +458,124 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,101 +857,779 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" customWidth="1"/>
+    <col min="11" max="11" width="24.5546875" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="108.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="F1" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="29"/>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="9">
+        <f>(E4-C4)/D4</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="J2" s="9">
+        <f>2/D4</f>
+        <v>2.6666666666666668E-2</v>
+      </c>
+      <c r="K2" s="4">
+        <f>1/D4</f>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="L2" s="4">
+        <f>(E4-C4-2)/D4</f>
+        <v>0.24</v>
+      </c>
+      <c r="M2" s="4">
+        <f>(D4-E4-2)/(D4-E4)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="6">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="6">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D3" s="6">
-        <v>420000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="124.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="25">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="6">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D4" s="6">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E4" s="6">
+        <v>70</v>
+      </c>
+      <c r="F4" s="8">
+        <f>(D4/$C4)*100</f>
+        <v>150</v>
+      </c>
+      <c r="G4" s="8">
+        <f>(E4/$C4)*100</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="26"/>
       <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="6">
+        <v>35</v>
+      </c>
+      <c r="D5" s="6">
+        <v>45</v>
+      </c>
+      <c r="E5" s="6">
+        <v>45</v>
+      </c>
+      <c r="F5" s="8">
+        <f>(D5/$C5)*100</f>
+        <v>128.57142857142858</v>
+      </c>
+      <c r="G5" s="8">
+        <f>(E5/$C5)*100</f>
+        <v>128.57142857142858</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="27"/>
+      <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6">
+        <v>30</v>
+      </c>
+      <c r="E6" s="6">
+        <v>25</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" ref="F6:G20" si="0">(D6/$C6)*100</f>
+        <v>200</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="0"/>
+        <v>166.66666666666669</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25">
         <v>2</v>
       </c>
-      <c r="D5" s="6">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6">
-        <f>SUM(D2:D5)</f>
-        <v>1070000</v>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6">
+        <v>50</v>
+      </c>
+      <c r="D7" s="6">
+        <v>75</v>
+      </c>
+      <c r="E7" s="6">
+        <v>70</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="26"/>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6">
+        <v>40</v>
+      </c>
+      <c r="D8" s="6">
+        <v>60</v>
+      </c>
+      <c r="E8" s="6">
+        <v>55</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="0"/>
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="46.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="26"/>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6">
+        <v>10</v>
+      </c>
+      <c r="E9" s="6">
+        <v>8</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>166.66666666666669</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="0"/>
+        <v>133.33333333333331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="67.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="27"/>
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6">
+        <v>7</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="110.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="25">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6">
+        <v>50</v>
+      </c>
+      <c r="D11" s="6">
+        <v>75</v>
+      </c>
+      <c r="E11" s="6">
+        <v>70</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="26"/>
+      <c r="B12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6">
+        <v>7</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="G12" s="8">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="26"/>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="6">
+        <v>15</v>
+      </c>
+      <c r="D13" s="6">
+        <v>40</v>
+      </c>
+      <c r="E13" s="6">
+        <v>30</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>266.66666666666663</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="26"/>
+      <c r="B14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="6">
+        <v>20</v>
+      </c>
+      <c r="D14" s="6">
+        <v>20</v>
+      </c>
+      <c r="E14" s="6">
+        <v>20</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G14" s="8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="27"/>
+      <c r="B15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="6">
+        <v>15</v>
+      </c>
+      <c r="D15" s="6">
+        <v>15</v>
+      </c>
+      <c r="E15" s="6">
+        <v>20</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G15" s="8">
+        <f t="shared" si="0"/>
+        <v>133.33333333333331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="94.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="25">
+        <v>4</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="6">
+        <v>50</v>
+      </c>
+      <c r="D16" s="6">
+        <v>75</v>
+      </c>
+      <c r="E16" s="6">
+        <v>70</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="G16" s="8">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="26"/>
+      <c r="B17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="6">
+        <v>10</v>
+      </c>
+      <c r="D17" s="6">
+        <v>18</v>
+      </c>
+      <c r="E17" s="6">
+        <v>17</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="G17" s="8">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="26"/>
+      <c r="B18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="6">
+        <v>15</v>
+      </c>
+      <c r="D18" s="6">
+        <v>20</v>
+      </c>
+      <c r="E18" s="6">
+        <v>18</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>133.33333333333331</v>
+      </c>
+      <c r="G18" s="8">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="27"/>
+      <c r="B19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="6">
+        <v>25</v>
+      </c>
+      <c r="D19" s="6">
+        <v>40</v>
+      </c>
+      <c r="E19" s="6">
+        <v>35</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="G19" s="8">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>5</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="6">
+        <v>45000</v>
+      </c>
+      <c r="D20" s="6">
+        <v>60000</v>
+      </c>
+      <c r="E20" s="6">
+        <v>55000</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
+        <v>133.33333333333331</v>
+      </c>
+      <c r="G20" s="8">
+        <f t="shared" si="0"/>
+        <v>122.22222222222223</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="11">
+        <v>65</v>
+      </c>
+      <c r="C2" s="16">
+        <v>70</v>
+      </c>
+      <c r="D2" s="20">
+        <f t="shared" ref="D2:D3" si="0">B2/C2</f>
+        <v>0.9285714285714286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="11">
+        <v>67</v>
+      </c>
+      <c r="C3" s="16">
+        <v>70</v>
+      </c>
+      <c r="D3" s="20">
+        <f t="shared" si="0"/>
+        <v>0.95714285714285718</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="21">
+        <f>AVERAGE(D2:D3)</f>
+        <v>0.94285714285714284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="13">
+        <v>40</v>
+      </c>
+      <c r="C6" s="16">
+        <v>70</v>
+      </c>
+      <c r="D6" s="20">
+        <f t="shared" ref="D6:D7" si="1">B6/C6</f>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="13">
+        <v>35</v>
+      </c>
+      <c r="C7" s="16">
+        <v>70</v>
+      </c>
+      <c r="D7" s="20">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="21">
+        <f>AVERAGE(D6:D7)</f>
+        <v>0.5357142857142857</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="23"/>
+    </row>
+    <row r="10" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="18">
+        <v>30</v>
+      </c>
+      <c r="C10" s="16">
+        <v>70</v>
+      </c>
+      <c r="D10" s="20">
+        <f t="shared" ref="D10:D11" si="2">B10/C10</f>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="18">
+        <v>27</v>
+      </c>
+      <c r="C11" s="16">
+        <v>70</v>
+      </c>
+      <c r="D11" s="20">
+        <f t="shared" si="2"/>
+        <v>0.38571428571428573</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="21">
+        <f>AVERAGE(D10:D11)</f>
+        <v>0.40714285714285714</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="37"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="38"/>
+    </row>
+    <row r="15" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="19">
+        <v>8</v>
+      </c>
+      <c r="C15" s="16">
+        <v>70</v>
+      </c>
+      <c r="D15" s="24">
+        <f t="shared" ref="D15:D16" si="3">B15/C15</f>
+        <v>0.11428571428571428</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="19">
+        <v>30</v>
+      </c>
+      <c r="C16" s="16">
+        <v>70</v>
+      </c>
+      <c r="D16" s="24">
+        <f t="shared" si="3"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="21">
+        <f>AVERAGE(D15:D16)</f>
+        <v>0.27142857142857141</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A13:B14"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:C12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>